<commit_message>
[ISP-2] Esportazione serie soriche per Punti di prelievo. Aggiunta serie
</commit_message>
<xml_diff>
--- a/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/10_LibFormula/10_LibFormula.xlsx
+++ b/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/10_LibFormula/10_LibFormula.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
   <si>
     <t>Action</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>TSLength</t>
+  </si>
+  <si>
+    <t>attributeExport</t>
+  </si>
+  <si>
+    <t>ExportUtils</t>
   </si>
 </sst>
 </file>
@@ -1253,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1324,6 +1330,14 @@
         <v>40</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1334,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1645,6 +1659,23 @@
       </c>
       <c r="F16" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1688,6 +1719,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1801,33 +1847,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1848,9 +1871,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>